<commit_message>
added toc and intro files
</commit_message>
<xml_diff>
--- a/data/observations_with_references.xlsx
+++ b/data/observations_with_references.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rla44\OneDrive\Github\UK-wood-mfa\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rla44\OneDrive\Github\UK-wood-end-use-flows\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A32C294-9F51-4C3F-9AE9-E6B71C11870C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9181F301-0E43-488A-8555-8BFB894D484E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="1000" xr2:uid="{7F14FEB3-C7FB-4348-9BE1-B4681E14C868}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{7F14FEB3-C7FB-4348-9BE1-B4681E14C868}"/>
   </bookViews>
   <sheets>
     <sheet name="Observations" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2528" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2529" uniqueCount="492">
   <si>
     <t>Region</t>
   </si>
@@ -1569,6 +1569,9 @@
   <si>
     <t>http://ukfires.org/probs/data/UK-wood/Observation-149</t>
   </si>
+  <si>
+    <t>CV_no_uncertainty</t>
+  </si>
 </sst>
 </file>
 
@@ -1580,7 +1583,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="General_)"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2659,7 +2662,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2791,6 +2794,7 @@
     <xf numFmtId="0" fontId="25" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3521,29 +3525,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D7DDC4-71AF-4822-B51E-055D7DEE741C}">
-  <dimension ref="A1:U126"/>
+  <dimension ref="A1:V126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
     <col min="7" max="7" width="31" style="90" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="44.140625" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="93"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>187</v>
       </c>
@@ -3601,14 +3606,17 @@
       <c r="S1" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="T1" s="32" t="s">
+      <c r="T1" s="25" t="s">
+        <v>491</v>
+      </c>
+      <c r="U1" s="32" t="s">
         <v>427</v>
       </c>
-      <c r="U1" s="32" t="s">
+      <c r="V1" s="32" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>188</v>
       </c>
@@ -3671,8 +3679,11 @@
         <f>R2/100</f>
         <v>5.0537115073973106E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="T2" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>189</v>
       </c>
@@ -3735,8 +3746,11 @@
         <f>R3/100</f>
         <v>5.0537115073973106E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="T3" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>190</v>
       </c>
@@ -3795,14 +3809,17 @@
         <v>5.0537115073973107</v>
       </c>
       <c r="S4" s="29">
-        <f t="shared" ref="S4:S65" si="2">R4/100</f>
+        <f t="shared" ref="S2:T65" si="2">R4/100</f>
         <v>5.0537115073973106E-2</v>
       </c>
-      <c r="T4" s="71" t="s">
+      <c r="T4" s="93">
+        <v>0</v>
+      </c>
+      <c r="U4" s="71" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>191</v>
       </c>
@@ -3864,11 +3881,14 @@
         <f t="shared" si="2"/>
         <v>5.0537115073973106E-2</v>
       </c>
-      <c r="T5" s="71" t="s">
+      <c r="T5" s="93">
+        <v>0</v>
+      </c>
+      <c r="U5" s="71" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>192</v>
       </c>
@@ -3930,11 +3950,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T6" s="71" t="s">
+      <c r="T6" s="93">
+        <v>0</v>
+      </c>
+      <c r="U6" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>193</v>
       </c>
@@ -3996,11 +4019,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T7" s="71" t="s">
+      <c r="T7" s="93">
+        <v>0</v>
+      </c>
+      <c r="U7" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="28" customFormat="1">
+    <row r="8" spans="1:22" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>194</v>
       </c>
@@ -4060,11 +4086,14 @@
         <f t="shared" si="2"/>
         <v>0.20600000000000002</v>
       </c>
-      <c r="T8" s="71" t="s">
+      <c r="T8" s="93">
+        <v>0</v>
+      </c>
+      <c r="U8" s="71" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="28" customFormat="1">
+    <row r="9" spans="1:22" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>195</v>
       </c>
@@ -4124,11 +4153,14 @@
         <f t="shared" si="2"/>
         <v>0.20600000000000002</v>
       </c>
-      <c r="T9" s="71" t="s">
+      <c r="T9" s="93">
+        <v>0</v>
+      </c>
+      <c r="U9" s="71" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="28" customFormat="1">
+    <row r="10" spans="1:22" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>196</v>
       </c>
@@ -4188,11 +4220,14 @@
         <f t="shared" si="2"/>
         <v>0.20600000000000002</v>
       </c>
-      <c r="T10" s="71" t="s">
+      <c r="T10" s="93">
+        <v>0</v>
+      </c>
+      <c r="U10" s="71" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="28" customFormat="1">
+    <row r="11" spans="1:22" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>197</v>
       </c>
@@ -4252,11 +4287,14 @@
         <f t="shared" si="2"/>
         <v>0.20600000000000002</v>
       </c>
-      <c r="T11" s="71" t="s">
+      <c r="T11" s="93">
+        <v>0</v>
+      </c>
+      <c r="U11" s="71" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>198</v>
       </c>
@@ -4315,11 +4353,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T12" s="71" t="s">
+      <c r="T12" s="93">
+        <v>0</v>
+      </c>
+      <c r="U12" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>199</v>
       </c>
@@ -4378,11 +4419,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T13" s="71" t="s">
+      <c r="T13" s="93">
+        <v>0</v>
+      </c>
+      <c r="U13" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>200</v>
       </c>
@@ -4441,11 +4485,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T14" s="71" t="s">
+      <c r="T14" s="93">
+        <v>0</v>
+      </c>
+      <c r="U14" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>201</v>
       </c>
@@ -4504,11 +4551,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T15" s="71" t="s">
+      <c r="T15" s="93">
+        <v>0</v>
+      </c>
+      <c r="U15" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>202</v>
       </c>
@@ -4567,11 +4617,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T16" s="71" t="s">
+      <c r="T16" s="93">
+        <v>0</v>
+      </c>
+      <c r="U16" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>203</v>
       </c>
@@ -4630,11 +4683,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T17" s="71" t="s">
+      <c r="T17" s="93">
+        <v>0</v>
+      </c>
+      <c r="U17" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>204</v>
       </c>
@@ -4693,11 +4749,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T18" s="71" t="s">
+      <c r="T18" s="93">
+        <v>0</v>
+      </c>
+      <c r="U18" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>205</v>
       </c>
@@ -4757,11 +4816,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T19" s="71" t="s">
+      <c r="T19" s="93">
+        <v>0</v>
+      </c>
+      <c r="U19" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>206</v>
       </c>
@@ -4820,11 +4882,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T20" s="71" t="s">
+      <c r="T20" s="93">
+        <v>0</v>
+      </c>
+      <c r="U20" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>207</v>
       </c>
@@ -4883,11 +4948,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T21" s="71" t="s">
+      <c r="T21" s="93">
+        <v>0</v>
+      </c>
+      <c r="U21" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>208</v>
       </c>
@@ -4946,11 +5014,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T22" s="71" t="s">
+      <c r="T22" s="93">
+        <v>0</v>
+      </c>
+      <c r="U22" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>209</v>
       </c>
@@ -5009,11 +5080,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T23" s="71" t="s">
+      <c r="T23" s="93">
+        <v>0</v>
+      </c>
+      <c r="U23" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>210</v>
       </c>
@@ -5072,11 +5146,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T24" s="71" t="s">
+      <c r="T24" s="93">
+        <v>0</v>
+      </c>
+      <c r="U24" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>211</v>
       </c>
@@ -5135,11 +5212,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T25" s="71" t="s">
+      <c r="T25" s="93">
+        <v>0</v>
+      </c>
+      <c r="U25" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>212</v>
       </c>
@@ -5201,11 +5281,14 @@
         <f t="shared" si="2"/>
         <v>0.15294770348063419</v>
       </c>
-      <c r="T26" s="71" t="s">
+      <c r="T26" s="93">
+        <v>0</v>
+      </c>
+      <c r="U26" s="71" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>213</v>
       </c>
@@ -5267,11 +5350,14 @@
         <f t="shared" si="2"/>
         <v>0.15294770348063419</v>
       </c>
-      <c r="T27" s="71" t="s">
+      <c r="T27" s="93">
+        <v>0</v>
+      </c>
+      <c r="U27" s="71" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>214</v>
       </c>
@@ -5333,11 +5419,14 @@
         <f t="shared" si="2"/>
         <v>0.15294770348063419</v>
       </c>
-      <c r="T28" s="71" t="s">
+      <c r="T28" s="93">
+        <v>0</v>
+      </c>
+      <c r="U28" s="71" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>215</v>
       </c>
@@ -5399,9 +5488,12 @@
         <f t="shared" si="2"/>
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="T29" s="71"/>
-    </row>
-    <row r="30" spans="1:20">
+      <c r="T29" s="93">
+        <v>0</v>
+      </c>
+      <c r="U29" s="71"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>216</v>
       </c>
@@ -5463,9 +5555,12 @@
         <f t="shared" si="2"/>
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="T30" s="71"/>
-    </row>
-    <row r="31" spans="1:20">
+      <c r="T30" s="93">
+        <v>0</v>
+      </c>
+      <c r="U30" s="71"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>217</v>
       </c>
@@ -5527,9 +5622,12 @@
         <f t="shared" si="2"/>
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="T31" s="71"/>
-    </row>
-    <row r="32" spans="1:20">
+      <c r="T31" s="93">
+        <v>0</v>
+      </c>
+      <c r="U31" s="71"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>218</v>
       </c>
@@ -5588,11 +5686,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T32" s="71" t="s">
+      <c r="T32" s="93">
+        <v>0</v>
+      </c>
+      <c r="U32" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>219</v>
       </c>
@@ -5651,11 +5752,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T33" s="71" t="s">
+      <c r="T33" s="93">
+        <v>0</v>
+      </c>
+      <c r="U33" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>220</v>
       </c>
@@ -5714,11 +5818,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T34" s="71" t="s">
+      <c r="T34" s="93">
+        <v>0</v>
+      </c>
+      <c r="U34" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>221</v>
       </c>
@@ -5777,11 +5884,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T35" s="71" t="s">
+      <c r="T35" s="93">
+        <v>0</v>
+      </c>
+      <c r="U35" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>222</v>
       </c>
@@ -5840,11 +5950,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T36" s="71" t="s">
+      <c r="T36" s="93">
+        <v>0</v>
+      </c>
+      <c r="U36" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>223</v>
       </c>
@@ -5903,11 +6016,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T37" s="71" t="s">
+      <c r="T37" s="93">
+        <v>0</v>
+      </c>
+      <c r="U37" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>224</v>
       </c>
@@ -5966,11 +6082,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T38" s="71" t="s">
+      <c r="T38" s="93">
+        <v>0</v>
+      </c>
+      <c r="U38" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>225</v>
       </c>
@@ -6029,11 +6148,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T39" s="71" t="s">
+      <c r="T39" s="93">
+        <v>0</v>
+      </c>
+      <c r="U39" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>226</v>
       </c>
@@ -6092,11 +6214,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T40" s="71" t="s">
+      <c r="T40" s="93">
+        <v>0</v>
+      </c>
+      <c r="U40" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>227</v>
       </c>
@@ -6158,11 +6283,14 @@
         <f t="shared" si="2"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T41" s="71" t="s">
+      <c r="T41" s="93">
+        <v>0</v>
+      </c>
+      <c r="U41" s="71" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>228</v>
       </c>
@@ -6221,11 +6349,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T42" s="71" t="s">
+      <c r="T42" s="93">
+        <v>0</v>
+      </c>
+      <c r="U42" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>229</v>
       </c>
@@ -6284,11 +6415,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T43" s="71" t="s">
+      <c r="T43" s="93">
+        <v>0</v>
+      </c>
+      <c r="U43" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>230</v>
       </c>
@@ -6347,11 +6481,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T44" s="71" t="s">
+      <c r="T44" s="93">
+        <v>0</v>
+      </c>
+      <c r="U44" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>231</v>
       </c>
@@ -6410,11 +6547,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T45" s="71" t="s">
+      <c r="T45" s="93">
+        <v>0</v>
+      </c>
+      <c r="U45" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>232</v>
       </c>
@@ -6473,11 +6613,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T46" s="71" t="s">
+      <c r="T46" s="93">
+        <v>0</v>
+      </c>
+      <c r="U46" s="71" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>233</v>
       </c>
@@ -6531,11 +6674,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T47" s="71" t="s">
+      <c r="T47" s="93">
+        <v>0</v>
+      </c>
+      <c r="U47" s="71" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>234</v>
       </c>
@@ -6597,11 +6743,14 @@
         <f t="shared" si="2"/>
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="T48" s="71" t="s">
+      <c r="T48" s="93">
+        <v>0</v>
+      </c>
+      <c r="U48" s="71" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>235</v>
       </c>
@@ -6663,11 +6812,14 @@
         <f t="shared" si="2"/>
         <v>0.15294770348063419</v>
       </c>
-      <c r="T49" t="s">
+      <c r="T49" s="93">
+        <v>0</v>
+      </c>
+      <c r="U49" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>236</v>
       </c>
@@ -6729,11 +6881,14 @@
         <f t="shared" si="2"/>
         <v>0.15294770348063419</v>
       </c>
-      <c r="T50" t="s">
+      <c r="T50" s="93">
+        <v>0</v>
+      </c>
+      <c r="U50" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>237</v>
       </c>
@@ -6755,8 +6910,11 @@
       <c r="S51" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:20">
+      <c r="T51" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>238</v>
       </c>
@@ -6818,11 +6976,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T52" t="s">
+      <c r="T52" s="93">
+        <v>0</v>
+      </c>
+      <c r="U52" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>239</v>
       </c>
@@ -6884,11 +7045,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T53" s="67" t="s">
+      <c r="T53" s="93">
+        <v>0</v>
+      </c>
+      <c r="U53" s="67" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>240</v>
       </c>
@@ -6947,11 +7111,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T54" s="67" t="s">
+      <c r="T54" s="93">
+        <v>0</v>
+      </c>
+      <c r="U54" s="67" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>241</v>
       </c>
@@ -7010,11 +7177,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T55" s="67" t="s">
+      <c r="T55" s="93">
+        <v>0</v>
+      </c>
+      <c r="U55" s="67" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>242</v>
       </c>
@@ -7076,11 +7246,14 @@
         <f t="shared" si="2"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T56" t="s">
+      <c r="T56" s="93">
+        <v>0</v>
+      </c>
+      <c r="U56" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>243</v>
       </c>
@@ -7142,11 +7315,14 @@
         <f t="shared" si="2"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T57" s="67" t="s">
+      <c r="T57" s="93">
+        <v>0</v>
+      </c>
+      <c r="U57" s="67" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>244</v>
       </c>
@@ -7206,11 +7382,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T58" s="67" t="s">
+      <c r="T58" s="93">
+        <v>0</v>
+      </c>
+      <c r="U58" s="67" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>245</v>
       </c>
@@ -7270,11 +7449,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T59" s="67" t="s">
+      <c r="T59" s="93">
+        <v>0</v>
+      </c>
+      <c r="U59" s="67" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>246</v>
       </c>
@@ -7334,11 +7516,14 @@
         <f t="shared" si="2"/>
         <v>0.14602397063496114</v>
       </c>
-      <c r="T60" s="73" t="s">
+      <c r="T60" s="93">
+        <v>0</v>
+      </c>
+      <c r="U60" s="73" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>247</v>
       </c>
@@ -7398,11 +7583,14 @@
         <f t="shared" si="2"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T61" s="67" t="s">
+      <c r="T61" s="93">
+        <v>0</v>
+      </c>
+      <c r="U61" s="67" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>248</v>
       </c>
@@ -7461,11 +7649,14 @@
         <f t="shared" si="2"/>
         <v>0.46152464722915937</v>
       </c>
-      <c r="T62" s="67" t="s">
+      <c r="T62" s="93">
+        <v>0</v>
+      </c>
+      <c r="U62" s="67" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>249</v>
       </c>
@@ -7524,11 +7715,14 @@
         <f t="shared" si="2"/>
         <v>0.46152464722915937</v>
       </c>
-      <c r="T63" s="67" t="s">
+      <c r="T63" s="93">
+        <v>0</v>
+      </c>
+      <c r="U63" s="67" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>250</v>
       </c>
@@ -7587,11 +7781,14 @@
         <f t="shared" si="2"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T64" t="s">
+      <c r="T64" s="93">
+        <v>0</v>
+      </c>
+      <c r="U64" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
         <v>251</v>
       </c>
@@ -7650,11 +7847,14 @@
         <f t="shared" si="2"/>
         <v>0.46152464722915937</v>
       </c>
-      <c r="T65" s="67" t="s">
+      <c r="T65" s="93">
+        <v>0</v>
+      </c>
+      <c r="U65" s="67" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
         <v>252</v>
       </c>
@@ -7713,11 +7913,14 @@
         <f t="shared" ref="S66:S93" si="4">R66/100</f>
         <v>0.46152464722915937</v>
       </c>
-      <c r="T66" s="86" t="s">
+      <c r="T66" s="93">
+        <v>0</v>
+      </c>
+      <c r="U66" s="86" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
         <v>253</v>
       </c>
@@ -7734,7 +7937,7 @@
         <v>39</v>
       </c>
       <c r="G67" s="90">
-        <f t="shared" ref="G67:G114" si="5">H67*1000</f>
+        <f t="shared" ref="G67:G113" si="5">H67*1000</f>
         <v>1936430.7280513917</v>
       </c>
       <c r="H67">
@@ -7776,11 +7979,14 @@
         <f t="shared" si="4"/>
         <v>0.41363994004447874</v>
       </c>
-      <c r="T67" t="s">
+      <c r="T67" s="93">
+        <v>0</v>
+      </c>
+      <c r="U67" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>254</v>
       </c>
@@ -7837,11 +8043,14 @@
         <f t="shared" si="4"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T68" t="s">
+      <c r="T68" s="93">
+        <v>0</v>
+      </c>
+      <c r="U68" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
         <v>255</v>
       </c>
@@ -7898,11 +8107,14 @@
         <f t="shared" si="4"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T69" s="67" t="s">
+      <c r="T69" s="93">
+        <v>0</v>
+      </c>
+      <c r="U69" s="67" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
         <v>256</v>
       </c>
@@ -7959,11 +8171,14 @@
         <f t="shared" si="4"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T70" s="67" t="s">
+      <c r="T70" s="93">
+        <v>0</v>
+      </c>
+      <c r="U70" s="67" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
         <v>257</v>
       </c>
@@ -8020,11 +8235,14 @@
         <f t="shared" si="4"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T71" s="67" t="s">
+      <c r="T71" s="93">
+        <v>0</v>
+      </c>
+      <c r="U71" s="67" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
         <v>258</v>
       </c>
@@ -8081,11 +8299,14 @@
         <f t="shared" si="4"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T72" s="67" t="s">
+      <c r="T72" s="93">
+        <v>0</v>
+      </c>
+      <c r="U72" s="67" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="73" spans="1:20">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
         <v>259</v>
       </c>
@@ -8142,11 +8363,14 @@
         <f t="shared" si="4"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T73" s="67" t="s">
+      <c r="T73" s="93">
+        <v>0</v>
+      </c>
+      <c r="U73" s="67" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="74" spans="1:20">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
         <v>260</v>
       </c>
@@ -8203,11 +8427,14 @@
         <f t="shared" si="4"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T74" s="67" t="s">
+      <c r="T74" s="93">
+        <v>0</v>
+      </c>
+      <c r="U74" s="67" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="75" spans="1:20">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>261</v>
       </c>
@@ -8261,8 +8488,11 @@
         <f t="shared" si="4"/>
         <v>2.3E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:20" s="67" customFormat="1">
+      <c r="T75" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
         <v>262</v>
       </c>
@@ -8295,8 +8525,11 @@
       <c r="S76" s="67">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:20">
+      <c r="T76" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
         <v>263</v>
       </c>
@@ -8355,11 +8588,14 @@
         <f t="shared" si="4"/>
         <v>5.0537115073973106E-2</v>
       </c>
-      <c r="T77" t="s">
+      <c r="T77" s="93">
+        <v>0</v>
+      </c>
+      <c r="U77" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="78" spans="1:20">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
         <v>264</v>
       </c>
@@ -8418,8 +8654,11 @@
         <f t="shared" si="4"/>
         <v>0.46152464722915937</v>
       </c>
-    </row>
-    <row r="79" spans="1:20">
+      <c r="T78" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
         <v>265</v>
       </c>
@@ -8478,8 +8717,11 @@
         <f t="shared" si="4"/>
         <v>0.46152464722915937</v>
       </c>
-    </row>
-    <row r="80" spans="1:20">
+      <c r="T79" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
         <v>266</v>
       </c>
@@ -8538,11 +8780,14 @@
         <f t="shared" si="4"/>
         <v>5.0537115073973106E-2</v>
       </c>
-      <c r="T80" s="67" t="s">
+      <c r="T80" s="93">
+        <v>0</v>
+      </c>
+      <c r="U80" s="67" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="81" spans="1:20">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
         <v>267</v>
       </c>
@@ -8602,11 +8847,14 @@
         <f t="shared" si="4"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T81" t="s">
+      <c r="T81" s="93">
+        <v>0</v>
+      </c>
+      <c r="U81" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="82" spans="1:20">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
         <v>410</v>
       </c>
@@ -8658,8 +8906,11 @@
         <f t="shared" ref="S82:S83" si="9">R82/100</f>
         <v>2.3E-2</v>
       </c>
-    </row>
-    <row r="83" spans="1:20" s="28" customFormat="1">
+      <c r="T82" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
         <v>412</v>
       </c>
@@ -8711,8 +8962,11 @@
         <f t="shared" si="9"/>
         <v>2.3E-2</v>
       </c>
-    </row>
-    <row r="84" spans="1:20" s="28" customFormat="1">
+      <c r="T83" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="14"/>
       <c r="G84" s="90"/>
       <c r="H84" s="1"/>
@@ -8726,8 +8980,11 @@
       <c r="P84" s="4"/>
       <c r="R84" s="16"/>
       <c r="S84" s="30"/>
-    </row>
-    <row r="85" spans="1:20">
+      <c r="T84" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
         <v>417</v>
       </c>
@@ -8788,11 +9045,14 @@
         <f t="shared" si="4"/>
         <v>0.14602397063496114</v>
       </c>
-      <c r="T85" s="72" t="s">
+      <c r="T85" s="93">
+        <v>0</v>
+      </c>
+      <c r="U85" s="72" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="86" spans="1:20">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
         <v>418</v>
       </c>
@@ -8853,11 +9113,14 @@
         <f t="shared" si="4"/>
         <v>0.14602397063496114</v>
       </c>
-      <c r="T86" s="72" t="s">
+      <c r="T86" s="93">
+        <v>0</v>
+      </c>
+      <c r="U86" s="72" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="87" spans="1:20">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
         <v>268</v>
       </c>
@@ -8918,11 +9181,14 @@
         <f t="shared" si="4"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T87" s="72" t="s">
+      <c r="T87" s="93">
+        <v>0</v>
+      </c>
+      <c r="U87" s="72" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="88" spans="1:20">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
         <v>269</v>
       </c>
@@ -8983,11 +9249,14 @@
         <f t="shared" si="4"/>
         <v>0.4637132734783424</v>
       </c>
-      <c r="T88" s="72" t="s">
+      <c r="T88" s="93">
+        <v>0</v>
+      </c>
+      <c r="U88" s="72" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="89" spans="1:20">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
         <v>419</v>
       </c>
@@ -9048,11 +9317,14 @@
         <f t="shared" si="4"/>
         <v>0.46152464722915937</v>
       </c>
-      <c r="T89" s="72" t="s">
+      <c r="T89" s="93">
+        <v>0</v>
+      </c>
+      <c r="U89" s="72" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="90" spans="1:20">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
         <v>270</v>
       </c>
@@ -9113,11 +9385,14 @@
         <f t="shared" si="4"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T90" s="72" t="s">
+      <c r="T90" s="93">
+        <v>0</v>
+      </c>
+      <c r="U90" s="72" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="91" spans="1:20">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
         <v>271</v>
       </c>
@@ -9178,11 +9453,14 @@
         <f t="shared" si="4"/>
         <v>0.46152464722915937</v>
       </c>
-      <c r="T91" s="72" t="s">
+      <c r="T91" s="93">
+        <v>0</v>
+      </c>
+      <c r="U91" s="72" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="92" spans="1:20">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
         <v>272</v>
       </c>
@@ -9243,11 +9521,14 @@
         <f t="shared" si="4"/>
         <v>0.46152464722915937</v>
       </c>
-      <c r="T92" s="72" t="s">
+      <c r="T92" s="93">
+        <v>0</v>
+      </c>
+      <c r="U92" s="72" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="93" spans="1:20">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
         <v>273</v>
       </c>
@@ -9308,11 +9589,14 @@
         <f t="shared" si="4"/>
         <v>0.14602397063496114</v>
       </c>
-      <c r="T93" s="72" t="s">
+      <c r="T93" s="93">
+        <v>0</v>
+      </c>
+      <c r="U93" s="72" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="94" spans="1:20">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
         <v>274</v>
       </c>
@@ -9373,11 +9657,14 @@
         <f t="shared" ref="S94" si="11">R94/100</f>
         <v>0.41608052105331722</v>
       </c>
-      <c r="T94" s="72" t="s">
+      <c r="T94" s="93">
+        <v>0</v>
+      </c>
+      <c r="U94" s="72" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="95" spans="1:20">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
         <v>275</v>
       </c>
@@ -9438,11 +9725,14 @@
         <f t="shared" ref="S95" si="13">R95/100</f>
         <v>5.0537115073973106E-2</v>
       </c>
-      <c r="T95" s="72" t="s">
+      <c r="T95" s="93">
+        <v>0</v>
+      </c>
+      <c r="U95" s="72" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="96" spans="1:20">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
         <v>276</v>
       </c>
@@ -9503,11 +9793,14 @@
         <f t="shared" ref="S96:S97" si="15">R96/100</f>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T96" s="67" t="s">
+      <c r="T96" s="93">
+        <v>0</v>
+      </c>
+      <c r="U96" s="67" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="97" spans="1:20">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
         <v>277</v>
       </c>
@@ -9568,11 +9861,14 @@
         <f t="shared" si="15"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T97" s="67" t="s">
+      <c r="T97" s="93">
+        <v>0</v>
+      </c>
+      <c r="U97" s="67" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="17.399999999999999" customHeight="1">
+    <row r="98" spans="1:21" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
         <v>278</v>
       </c>
@@ -9633,11 +9929,14 @@
         <f t="shared" ref="S98:S101" si="17">R98/100</f>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T98" s="67" t="s">
+      <c r="T98" s="93">
+        <v>0</v>
+      </c>
+      <c r="U98" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="99" spans="1:20" s="59" customFormat="1" ht="17.399999999999999" customHeight="1">
+    <row r="99" spans="1:21" s="59" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
         <v>279</v>
       </c>
@@ -9698,11 +9997,14 @@
         <f t="shared" ref="S99" si="19">R99/100</f>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T99" s="67" t="s">
+      <c r="T99" s="93">
+        <v>0</v>
+      </c>
+      <c r="U99" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="100" spans="1:20">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
         <v>420</v>
       </c>
@@ -9763,11 +10065,14 @@
         <f t="shared" si="17"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T100" s="67" t="s">
+      <c r="T100" s="93">
+        <v>0</v>
+      </c>
+      <c r="U100" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="101" spans="1:20">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
         <v>356</v>
       </c>
@@ -9828,11 +10133,14 @@
         <f t="shared" si="17"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T101" s="67" t="s">
+      <c r="T101" s="93">
+        <v>0</v>
+      </c>
+      <c r="U101" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="102" spans="1:20">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
         <v>371</v>
       </c>
@@ -9895,11 +10203,14 @@
         <f t="shared" ref="S102" si="21">R102/100</f>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T102" s="67" t="s">
+      <c r="T102" s="93">
+        <v>0</v>
+      </c>
+      <c r="U102" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="103" spans="1:20">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
         <v>383</v>
       </c>
@@ -9960,11 +10271,14 @@
         <f t="shared" ref="S103:S104" si="23">R103/100</f>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T103" s="67" t="s">
+      <c r="T103" s="93">
+        <v>0</v>
+      </c>
+      <c r="U103" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="104" spans="1:20">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
         <v>386</v>
       </c>
@@ -10025,11 +10339,14 @@
         <f t="shared" si="23"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T104" s="67" t="s">
+      <c r="T104" s="93">
+        <v>0</v>
+      </c>
+      <c r="U104" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="105" spans="1:20">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
         <v>388</v>
       </c>
@@ -10090,11 +10407,14 @@
         <f t="shared" ref="S105:S108" si="25">R105/100</f>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T105" s="67" t="s">
+      <c r="T105" s="93">
+        <v>0</v>
+      </c>
+      <c r="U105" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="106" spans="1:20">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
         <v>390</v>
       </c>
@@ -10155,11 +10475,14 @@
         <f t="shared" si="25"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T106" s="67" t="s">
+      <c r="T106" s="93">
+        <v>0</v>
+      </c>
+      <c r="U106" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="107" spans="1:20">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
         <v>391</v>
       </c>
@@ -10220,11 +10543,14 @@
         <f t="shared" si="25"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T107" s="67" t="s">
+      <c r="T107" s="93">
+        <v>0</v>
+      </c>
+      <c r="U107" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="108" spans="1:20">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
         <v>392</v>
       </c>
@@ -10285,11 +10611,14 @@
         <f t="shared" si="25"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T108" s="67" t="s">
+      <c r="T108" s="93">
+        <v>0</v>
+      </c>
+      <c r="U108" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="109" spans="1:20">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
         <v>393</v>
       </c>
@@ -10350,11 +10679,14 @@
         <f t="shared" ref="S109:S111" si="27">R109/100</f>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T109" s="67" t="s">
+      <c r="T109" s="93">
+        <v>0</v>
+      </c>
+      <c r="U109" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="110" spans="1:20">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
         <v>397</v>
       </c>
@@ -10415,11 +10747,14 @@
         <f t="shared" si="27"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T110" s="67" t="s">
+      <c r="T110" s="93">
+        <v>0</v>
+      </c>
+      <c r="U110" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="111" spans="1:20">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
         <v>398</v>
       </c>
@@ -10480,11 +10815,14 @@
         <f t="shared" si="27"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T111" s="67" t="s">
+      <c r="T111" s="93">
+        <v>0</v>
+      </c>
+      <c r="U111" s="67" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="112" spans="1:20">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
         <v>399</v>
       </c>
@@ -10530,18 +10868,21 @@
         <v>0</v>
       </c>
       <c r="R112" s="16">
-        <f t="shared" ref="R112:R125" si="28">SQRT(M112^2+N112^2+O112^2+P112^2+Q112^2)</f>
+        <f t="shared" ref="R112:R124" si="28">SQRT(M112^2+N112^2+O112^2+P112^2+Q112^2)</f>
         <v>13.891724155050012</v>
       </c>
       <c r="S112" s="92">
-        <f t="shared" ref="S112:S125" si="29">R112/100</f>
+        <f t="shared" ref="S112:S124" si="29">R112/100</f>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T112" t="s">
+      <c r="T112" s="93">
+        <v>0</v>
+      </c>
+      <c r="U112" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="113" spans="1:20">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
         <v>400</v>
       </c>
@@ -10594,11 +10935,14 @@
         <f t="shared" si="29"/>
         <v>0.13891724155050011</v>
       </c>
-      <c r="T113" t="s">
+      <c r="T113" s="93">
+        <v>0</v>
+      </c>
+      <c r="U113" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="114" spans="1:20">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
         <v>479</v>
       </c>
@@ -10648,9 +10992,12 @@
         <f t="shared" si="29"/>
         <v>2.3E-2</v>
       </c>
-      <c r="T114" s="84"/>
-    </row>
-    <row r="115" spans="1:20">
+      <c r="T114" s="93">
+        <v>0</v>
+      </c>
+      <c r="U114" s="84"/>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
         <v>480</v>
       </c>
@@ -10700,8 +11047,11 @@
         <f t="shared" si="29"/>
         <v>2.3E-2</v>
       </c>
-    </row>
-    <row r="116" spans="1:20">
+      <c r="T115" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
         <v>481</v>
       </c>
@@ -10748,8 +11098,11 @@
         <f t="shared" si="29"/>
         <v>0.13891724155050011</v>
       </c>
-    </row>
-    <row r="117" spans="1:20">
+      <c r="T116" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
         <v>482</v>
       </c>
@@ -10796,8 +11149,11 @@
         <f t="shared" si="29"/>
         <v>0.13891724155050011</v>
       </c>
-    </row>
-    <row r="118" spans="1:20">
+      <c r="T117" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
         <v>483</v>
       </c>
@@ -10844,8 +11200,11 @@
         <f t="shared" si="29"/>
         <v>0.13891724155050011</v>
       </c>
-    </row>
-    <row r="119" spans="1:20">
+      <c r="T118" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
         <v>484</v>
       </c>
@@ -10892,8 +11251,11 @@
         <f t="shared" si="29"/>
         <v>0.13891724155050011</v>
       </c>
-    </row>
-    <row r="120" spans="1:20">
+      <c r="T119" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
         <v>485</v>
       </c>
@@ -10940,8 +11302,11 @@
         <f t="shared" si="29"/>
         <v>0.13891724155050011</v>
       </c>
-    </row>
-    <row r="121" spans="1:20">
+      <c r="T120" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
         <v>486</v>
       </c>
@@ -10988,8 +11353,11 @@
         <f t="shared" si="29"/>
         <v>0.13891724155050011</v>
       </c>
-    </row>
-    <row r="122" spans="1:20">
+      <c r="T121" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
         <v>487</v>
       </c>
@@ -11036,8 +11404,11 @@
         <f t="shared" si="29"/>
         <v>0.13891724155050011</v>
       </c>
-    </row>
-    <row r="123" spans="1:20">
+      <c r="T122" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
         <v>488</v>
       </c>
@@ -11084,8 +11455,11 @@
         <f t="shared" si="29"/>
         <v>0.13891724155050011</v>
       </c>
-    </row>
-    <row r="124" spans="1:20">
+      <c r="T123" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
         <v>489</v>
       </c>
@@ -11132,8 +11506,11 @@
         <f t="shared" si="29"/>
         <v>3.2526911934581182E-2</v>
       </c>
-    </row>
-    <row r="125" spans="1:20">
+      <c r="T124" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
         <v>490</v>
       </c>
@@ -11178,8 +11555,11 @@
       <c r="S125" s="92">
         <v>3.2526911934581182E-2</v>
       </c>
-    </row>
-    <row r="126" spans="1:20">
+      <c r="T125" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A126" s="14"/>
       <c r="B126" s="92"/>
       <c r="C126" s="92"/>
@@ -11218,23 +11598,23 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" style="85" customWidth="1"/>
-    <col min="7" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="59" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="59" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" style="85" customWidth="1"/>
+    <col min="7" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="59" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="59" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.109375" style="85" customWidth="1"/>
+    <col min="12" max="13" width="11.140625" style="85" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" style="20" customWidth="1"/>
     <col min="17" max="17" width="10" style="53" customWidth="1"/>
     <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -11290,7 +11670,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="14.4" customHeight="1">
+    <row r="2" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
         <v>458</v>
       </c>
@@ -11343,7 +11723,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="14.4" customHeight="1">
+    <row r="3" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
         <v>457</v>
       </c>
@@ -11396,7 +11776,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="36" customFormat="1" ht="14.4" customHeight="1">
+    <row r="4" spans="1:18" s="36" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="68" t="s">
         <v>456</v>
       </c>
@@ -11451,7 +11831,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="36" customFormat="1" ht="14.4" customHeight="1">
+    <row r="5" spans="1:18" s="36" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
         <v>455</v>
       </c>
@@ -11506,7 +11886,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="20.399999999999999" customHeight="1">
+    <row r="6" spans="1:18" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="69" t="s">
         <v>454</v>
       </c>
@@ -11558,7 +11938,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="16.2" customHeight="1">
+    <row r="7" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="70" t="s">
         <v>453</v>
       </c>
@@ -11610,7 +11990,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D8" s="7"/>
       <c r="E8" s="7">
         <f t="shared" si="1"/>
@@ -11626,7 +12006,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -11679,7 +12059,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -11732,7 +12112,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -11791,7 +12171,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -11850,7 +12230,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -11903,7 +12283,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>101</v>
       </c>
@@ -11956,7 +12336,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>102</v>
       </c>
@@ -12009,7 +12389,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -12062,7 +12442,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -12115,7 +12495,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -12168,7 +12548,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -12221,7 +12601,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>104</v>
       </c>
@@ -12274,7 +12654,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>104</v>
       </c>
@@ -12327,7 +12707,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D22" s="7"/>
       <c r="E22" s="7">
         <f t="shared" si="1"/>
@@ -12344,7 +12724,7 @@
       </c>
       <c r="R22" s="9"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="67" t="s">
         <v>402</v>
       </c>
@@ -12377,7 +12757,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="67" t="s">
         <v>402</v>
       </c>
@@ -12410,7 +12790,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="67" t="s">
         <v>403</v>
       </c>
@@ -12443,7 +12823,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="67" t="s">
         <v>403</v>
       </c>
@@ -12476,7 +12856,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="67" t="s">
         <v>404</v>
       </c>
@@ -12509,7 +12889,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="67" t="s">
         <v>404</v>
       </c>
@@ -12542,7 +12922,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="67" t="s">
         <v>405</v>
       </c>
@@ -12575,7 +12955,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="67" t="s">
         <v>405</v>
       </c>
@@ -12608,7 +12988,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L31" s="85" t="s">
         <v>105</v>
       </c>
@@ -12633,17 +13013,17 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.44140625" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
     <col min="2" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="53"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -12676,7 +13056,7 @@
       </c>
       <c r="K1" s="25"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
         <v>459</v>
       </c>
@@ -12709,7 +13089,7 @@
       </c>
       <c r="K2" s="14"/>
     </row>
-    <row r="3" spans="1:12" ht="14.4" customHeight="1">
+    <row r="3" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
         <v>460</v>
       </c>
@@ -12734,17 +13114,17 @@
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1">
+    <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="68"/>
       <c r="K4" s="14"/>
     </row>
-    <row r="5" spans="1:12" s="36" customFormat="1" ht="14.4" customHeight="1">
+    <row r="5" spans="1:12" s="36" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J5" s="53"/>
     </row>
-    <row r="6" spans="1:12" s="36" customFormat="1" ht="14.4" customHeight="1">
+    <row r="6" spans="1:12" s="36" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J6" s="53"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -12777,7 +13157,7 @@
       </c>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -12810,7 +13190,7 @@
       </c>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -12843,7 +13223,7 @@
       </c>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -12876,7 +13256,7 @@
       </c>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -12909,7 +13289,7 @@
       </c>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -12942,7 +13322,7 @@
       </c>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>408</v>
       </c>
@@ -12962,7 +13342,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>408</v>
       </c>
@@ -12982,7 +13362,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="53"/>
       <c r="B15" s="67"/>
       <c r="C15" s="67"/>
@@ -12990,20 +13370,20 @@
       <c r="E15" s="65"/>
       <c r="F15" s="67"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="67"/>
       <c r="C16" s="67"/>
       <c r="D16" s="65"/>
       <c r="E16" s="65"/>
       <c r="F16" s="67"/>
     </row>
-    <row r="17" spans="5:5">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17">
         <f>E9+E11</f>
         <v>38518302</v>
       </c>
     </row>
-    <row r="18" spans="5:5">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="91">
         <f>E10+E12</f>
         <v>5278902</v>
@@ -13024,16 +13404,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -13075,7 +13455,7 @@
       <c r="S1" s="32"/>
       <c r="T1" s="32"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>465</v>
       </c>
@@ -13109,7 +13489,7 @@
       <c r="S2" s="18"/>
       <c r="T2" s="80"/>
     </row>
-    <row r="3" spans="1:20" s="67" customFormat="1">
+    <row r="3" spans="1:20" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77"/>
       <c r="B3" s="77"/>
       <c r="C3" s="77"/>
@@ -13131,7 +13511,7 @@
       <c r="S3" s="18"/>
       <c r="T3" s="80"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="76" t="s">
         <v>465</v>
       </c>
@@ -13165,7 +13545,7 @@
       <c r="S4" s="18"/>
       <c r="T4" s="18"/>
     </row>
-    <row r="5" spans="1:20" s="67" customFormat="1">
+    <row r="5" spans="1:20" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="76" t="s">
         <v>465</v>
       </c>
@@ -13199,7 +13579,7 @@
       <c r="S5" s="18"/>
       <c r="T5" s="18"/>
     </row>
-    <row r="6" spans="1:20" s="67" customFormat="1">
+    <row r="6" spans="1:20" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="77"/>
       <c r="B6" s="77"/>
       <c r="C6" s="77"/>
@@ -13221,7 +13601,7 @@
       <c r="S6" s="18"/>
       <c r="T6" s="18"/>
     </row>
-    <row r="7" spans="1:20" s="67" customFormat="1">
+    <row r="7" spans="1:20" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="77"/>
       <c r="B7" s="77"/>
       <c r="C7" s="77"/>
@@ -13243,7 +13623,7 @@
       <c r="S7" s="18"/>
       <c r="T7" s="18"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="82"/>
       <c r="B8" s="82"/>
       <c r="C8" s="82"/>
@@ -13265,7 +13645,7 @@
       <c r="S8" s="18"/>
       <c r="T8" s="18"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="77"/>
       <c r="B9" s="77"/>
       <c r="C9" s="77"/>
@@ -13287,7 +13667,7 @@
       <c r="S9" s="18"/>
       <c r="T9" s="18"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="77"/>
       <c r="B10" s="77"/>
       <c r="C10" s="77"/>
@@ -13309,7 +13689,7 @@
       <c r="S10" s="18"/>
       <c r="T10" s="18"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="75"/>
       <c r="B11" s="75"/>
       <c r="C11" s="75"/>
@@ -13327,7 +13707,7 @@
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
@@ -13356,16 +13736,16 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="14.33203125" style="85" customWidth="1"/>
-    <col min="9" max="10" width="8.88671875" style="55"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="14.28515625" style="85" customWidth="1"/>
+    <col min="9" max="10" width="8.85546875" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -13397,7 +13777,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>5</v>
       </c>
@@ -13430,7 +13810,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>5</v>
       </c>
@@ -13463,7 +13843,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="85" t="s">
         <v>5</v>
       </c>
@@ -13491,44 +13871,44 @@
       </c>
       <c r="J4" s="16"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E5" s="24"/>
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
       <c r="J5" s="16"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J6" s="16"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J7" s="16"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J8" s="16"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J10" s="16"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J16" s="16"/>
     </row>
   </sheetData>
@@ -13544,17 +13924,17 @@
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="3" max="9" width="9.109375" customWidth="1"/>
-    <col min="10" max="10" width="64.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="3" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="64.28515625" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" style="20" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>110</v>
       </c>
@@ -13583,19 +13963,19 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="94" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="95" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
       <c r="K2" s="20">
         <v>2019</v>
       </c>
@@ -13615,7 +13995,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>165</v>
       </c>
@@ -13637,7 +14017,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -13662,13 +14042,13 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
       <c r="O5" s="20"/>
       <c r="P5" s="20"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>168</v>
       </c>
@@ -13685,7 +14065,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>168</v>
       </c>
@@ -13702,7 +14082,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>168</v>
       </c>
@@ -13720,7 +14100,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -13755,12 +14135,12 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -13795,7 +14175,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -13829,7 +14209,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
@@ -13863,7 +14243,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
@@ -13897,7 +14277,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -13931,7 +14311,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -13965,7 +14345,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
@@ -13999,7 +14379,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
@@ -14033,7 +14413,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="36" customFormat="1" ht="15" thickBot="1">
+    <row r="10" spans="1:19" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>0</v>
       </c>
@@ -14068,7 +14448,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>5</v>
       </c>
@@ -14103,7 +14483,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>5</v>
       </c>
@@ -14138,7 +14518,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>5</v>
       </c>
@@ -14173,7 +14553,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>5</v>
       </c>
@@ -14208,7 +14588,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>5</v>
       </c>
@@ -14273,18 +14653,18 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" style="85" customWidth="1"/>
-    <col min="12" max="12" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" style="85" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
@@ -14293,7 +14673,7 @@
     <col min="19" max="19" width="10" style="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" thickBot="1">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -14336,10 +14716,10 @@
       <c r="N1" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="O1" s="93" t="s">
+      <c r="O1" s="94" t="s">
         <v>152</v>
       </c>
-      <c r="P1" s="93"/>
+      <c r="P1" s="94"/>
       <c r="Q1" s="25" t="s">
         <v>299</v>
       </c>
@@ -14359,7 +14739,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -14427,7 +14807,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -14495,7 +14875,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -14563,7 +14943,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -14631,7 +15011,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -14699,7 +15079,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -14767,7 +15147,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -14835,7 +15215,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="13.95" customHeight="1">
+    <row r="9" spans="1:22" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -14903,7 +15283,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="21" customFormat="1">
+    <row r="10" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>5</v>
       </c>
@@ -14971,7 +15351,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="21" customFormat="1">
+    <row r="11" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>5</v>
       </c>
@@ -15039,7 +15419,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="53" customFormat="1">
+    <row r="12" spans="1:22" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>5</v>
       </c>
@@ -15107,7 +15487,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="21" customFormat="1">
+    <row r="13" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>5</v>
       </c>
@@ -15175,7 +15555,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="21" customFormat="1">
+    <row r="14" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>5</v>
       </c>
@@ -15243,7 +15623,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="21" customFormat="1">
+    <row r="15" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>5</v>
       </c>
@@ -15311,7 +15691,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="21" customFormat="1">
+    <row r="16" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>5</v>
       </c>
@@ -15379,30 +15759,30 @@
         <v>352</v>
       </c>
     </row>
-    <row r="18" spans="6:7">
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F18" s="20"/>
     </row>
-    <row r="19" spans="6:7">
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F19" s="20"/>
     </row>
-    <row r="20" spans="6:7">
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F20" s="20"/>
       <c r="G20" s="27"/>
     </row>
-    <row r="21" spans="6:7">
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F21" s="20"/>
       <c r="G21" s="27"/>
     </row>
-    <row r="22" spans="6:7">
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F22" s="20"/>
     </row>
-    <row r="23" spans="6:7">
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F23" s="20"/>
     </row>
-    <row r="24" spans="6:7">
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F24" s="20"/>
     </row>
-    <row r="25" spans="6:7">
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F25" s="20"/>
     </row>
   </sheetData>
@@ -15426,30 +15806,30 @@
       <selection activeCell="G2" sqref="G2:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5546875" style="85" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5546875" style="20" customWidth="1"/>
-    <col min="15" max="15" width="23.109375" style="20" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" style="20" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="85" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5703125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" style="20" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="20" customWidth="1"/>
     <col min="18" max="18" width="8" style="20" customWidth="1"/>
-    <col min="19" max="19" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5546875" style="20" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" style="20" customWidth="1"/>
-    <col min="22" max="22" width="9.44140625" style="20" customWidth="1"/>
+    <col min="19" max="19" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" style="20" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" style="20" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1">
+    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -15498,7 +15878,7 @@
       <c r="V1" s="10"/>
       <c r="W1" s="32"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -15547,7 +15927,7 @@
       <c r="U2" s="16"/>
       <c r="V2" s="16"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -15597,7 +15977,7 @@
       <c r="V3" s="16"/>
       <c r="W3" s="36"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -15644,7 +16024,7 @@
       <c r="V4" s="16"/>
       <c r="W4" s="36"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -15691,7 +16071,7 @@
       <c r="V5" s="16"/>
       <c r="W5" s="36"/>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -15738,7 +16118,7 @@
       <c r="V6" s="16"/>
       <c r="W6" s="36"/>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -15785,7 +16165,7 @@
       <c r="V7" s="16"/>
       <c r="W7" s="36"/>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
@@ -15793,7 +16173,7 @@
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
     </row>
-    <row r="10" spans="1:23" ht="17.399999999999999">
+    <row r="10" spans="1:23" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="74"/>
       <c r="B10" s="74"/>
       <c r="C10" s="74"/>
@@ -15801,7 +16181,7 @@
       <c r="E10" s="74"/>
       <c r="F10" s="24"/>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
@@ -15823,22 +16203,22 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="85" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="85" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -15881,10 +16261,10 @@
       <c r="N1" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="O1" s="93" t="s">
+      <c r="O1" s="94" t="s">
         <v>152</v>
       </c>
-      <c r="P1" s="93"/>
+      <c r="P1" s="94"/>
       <c r="Q1" s="25" t="s">
         <v>293</v>
       </c>
@@ -15898,7 +16278,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
@@ -15963,7 +16343,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
@@ -16028,7 +16408,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>5</v>
       </c>
@@ -16093,40 +16473,40 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="39" customFormat="1">
+    <row r="5" spans="1:20" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F5" s="1"/>
       <c r="K5" s="85"/>
       <c r="N5" s="1"/>
       <c r="P5" s="32"/>
     </row>
-    <row r="6" spans="1:20" s="39" customFormat="1">
+    <row r="6" spans="1:20" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F6" s="1"/>
       <c r="K6" s="85"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="Q6" s="16"/>
     </row>
-    <row r="7" spans="1:20" s="39" customFormat="1">
+    <row r="7" spans="1:20" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F7" s="1"/>
       <c r="K7" s="85"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="Q7" s="16"/>
     </row>
-    <row r="8" spans="1:20" s="30" customFormat="1">
+    <row r="8" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F8" s="1"/>
       <c r="K8" s="85"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="Q8" s="16"/>
     </row>
-    <row r="9" spans="1:20" s="30" customFormat="1">
+    <row r="9" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K9" s="85"/>
       <c r="M9" s="1"/>
       <c r="O9" s="1"/>
       <c r="Q9" s="16"/>
     </row>
-    <row r="10" spans="1:20" s="30" customFormat="1" ht="15" thickBot="1">
+    <row r="10" spans="1:20" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>0</v>
       </c>
@@ -16172,7 +16552,7 @@
       </c>
       <c r="Q10" s="16"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>5</v>
       </c>
@@ -16224,7 +16604,7 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="14"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
@@ -16236,12 +16616,12 @@
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="P15" s="20"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="20"/>
     </row>
-    <row r="16" spans="1:20" ht="15" thickBot="1">
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>0</v>
       </c>
@@ -16286,7 +16666,7 @@
       <c r="Q16" s="20"/>
       <c r="R16" s="20"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
@@ -16356,17 +16736,17 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="85"/>
-    <col min="10" max="10" width="14.5546875" customWidth="1"/>
-    <col min="11" max="11" width="7.88671875" style="36" customWidth="1"/>
-    <col min="12" max="13" width="9.6640625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="85"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="36" customWidth="1"/>
+    <col min="12" max="13" width="9.7109375" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -16413,7 +16793,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -16459,7 +16839,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -16502,7 +16882,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -16545,7 +16925,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -16588,7 +16968,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -16634,7 +17014,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -16677,7 +17057,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -16720,7 +17100,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -16763,7 +17143,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -16806,7 +17186,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -16862,19 +17242,19 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" style="85" customWidth="1"/>
-    <col min="13" max="13" width="20.5546875" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="34"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="85" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="34"/>
     <col min="15" max="15" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="20" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:19" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -16930,7 +17310,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
@@ -16988,7 +17368,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
@@ -17045,7 +17425,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>5</v>
       </c>
@@ -17102,7 +17482,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>5</v>
       </c>
@@ -17159,7 +17539,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>5</v>
       </c>
@@ -17217,7 +17597,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
@@ -17274,7 +17654,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>5</v>
       </c>
@@ -17331,7 +17711,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>5</v>
       </c>
@@ -17388,7 +17768,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>5</v>
       </c>
@@ -17446,7 +17826,7 @@
       </c>
       <c r="S10" s="56"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>5</v>
       </c>
@@ -17505,7 +17885,7 @@
       </c>
       <c r="S11" s="56"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
@@ -17562,7 +17942,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>5</v>
       </c>
@@ -17619,7 +17999,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>5</v>
       </c>
@@ -17676,7 +18056,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>5</v>
       </c>
@@ -17735,7 +18115,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>5</v>
       </c>
@@ -17792,7 +18172,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
@@ -17866,28 +18246,28 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="10" style="85" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="85"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" style="85" customWidth="1"/>
-    <col min="11" max="12" width="12.44140625" style="59" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" style="85" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" style="36"/>
-    <col min="17" max="17" width="8.88671875" style="30"/>
+    <col min="6" max="6" width="9.140625" style="85"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="85" customWidth="1"/>
+    <col min="11" max="12" width="12.42578125" style="59" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" style="85" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="36"/>
+    <col min="17" max="17" width="8.85546875" style="30"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.33203125" customWidth="1"/>
-    <col min="20" max="20" width="8.44140625" style="36" customWidth="1"/>
-    <col min="21" max="21" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" style="36" customWidth="1"/>
+    <col min="21" max="21" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="11" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" thickBot="1">
+    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -17942,10 +18322,10 @@
       <c r="R1" s="25" t="s">
         <v>444</v>
       </c>
-      <c r="S1" s="93" t="s">
+      <c r="S1" s="94" t="s">
         <v>288</v>
       </c>
-      <c r="T1" s="93"/>
+      <c r="T1" s="94"/>
       <c r="U1" s="10" t="s">
         <v>63</v>
       </c>
@@ -17958,12 +18338,12 @@
       <c r="X1" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="Y1" s="93" t="s">
+      <c r="Y1" s="94" t="s">
         <v>288</v>
       </c>
-      <c r="Z1" s="93"/>
-    </row>
-    <row r="2" spans="1:26" ht="14.4" customHeight="1">
+      <c r="Z1" s="94"/>
+    </row>
+    <row r="2" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
         <v>344</v>
       </c>
@@ -18045,7 +18425,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.4" customHeight="1">
+    <row r="3" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
         <v>345</v>
       </c>
@@ -18127,7 +18507,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.4" customHeight="1">
+    <row r="4" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="68" t="s">
         <v>113</v>
       </c>
@@ -18207,7 +18587,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.4" customHeight="1">
+    <row r="5" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
         <v>374</v>
       </c>
@@ -18287,7 +18667,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.4" customHeight="1">
+    <row r="6" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="68" t="s">
         <v>346</v>
       </c>
@@ -18367,7 +18747,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.4" customHeight="1">
+    <row r="7" spans="1:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="68" t="s">
         <v>355</v>
       </c>
@@ -18446,7 +18826,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="I8" s="85"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -18455,7 +18835,7 @@
       <c r="S8" s="14"/>
       <c r="T8" s="14"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="I9" s="85"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -18464,7 +18844,7 @@
       <c r="S9" s="14"/>
       <c r="T9" s="14"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>375</v>
       </c>
@@ -18519,7 +18899,7 @@
       <c r="S10" s="14"/>
       <c r="T10" s="14"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>375</v>
       </c>
@@ -18578,7 +18958,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>376</v>
       </c>
@@ -18640,7 +19020,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>376</v>
       </c>
@@ -18702,7 +19082,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>92</v>
       </c>
@@ -18768,7 +19148,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>92</v>
       </c>
@@ -18834,7 +19214,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>113</v>
       </c>
@@ -18899,7 +19279,7 @@
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -18964,13 +19344,13 @@
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="57"/>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
     </row>
   </sheetData>
@@ -18995,23 +19375,23 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="80" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.33203125" style="85" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="53" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="53" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" style="85" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.28515625" style="85" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="53" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="53" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="85" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -19058,7 +19438,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="14.4" customHeight="1">
+    <row r="2" spans="1:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
         <v>445</v>
       </c>
@@ -19108,7 +19488,7 @@
         <v>106097400</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
         <v>446</v>
       </c>
@@ -19161,7 +19541,7 @@
       <c r="Q3" s="59"/>
       <c r="R3" s="59"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="68" t="s">
         <v>447</v>
       </c>
@@ -19214,7 +19594,7 @@
       <c r="Q4" s="59"/>
       <c r="R4" s="59"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
         <v>448</v>
       </c>
@@ -19267,7 +19647,7 @@
       <c r="Q5" s="59"/>
       <c r="R5" s="59"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="68" t="s">
         <v>449</v>
       </c>
@@ -19320,7 +19700,7 @@
       <c r="Q6" s="59"/>
       <c r="R6" s="59"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="68" t="s">
         <v>450</v>
       </c>
@@ -19373,7 +19753,7 @@
       <c r="Q7" s="59"/>
       <c r="R7" s="59"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="68" t="s">
         <v>451</v>
       </c>
@@ -19426,7 +19806,7 @@
       <c r="Q8" s="59"/>
       <c r="R8" s="59"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -19444,7 +19824,7 @@
       <c r="Q9" s="59"/>
       <c r="R9" s="59"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -19481,7 +19861,7 @@
       </c>
       <c r="L12" s="34"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -19518,7 +19898,7 @@
       </c>
       <c r="L13" s="34"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -19555,7 +19935,7 @@
       </c>
       <c r="L14" s="34"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -19592,7 +19972,7 @@
       </c>
       <c r="L15" s="34"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -19629,7 +20009,7 @@
       </c>
       <c r="L16" s="34"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -19666,7 +20046,7 @@
       </c>
       <c r="L17" s="34"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -19703,7 +20083,7 @@
       </c>
       <c r="L18" s="34"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -19740,7 +20120,7 @@
       </c>
       <c r="L19" s="34"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -19777,7 +20157,7 @@
       </c>
       <c r="L20" s="34"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -19814,7 +20194,7 @@
       </c>
       <c r="L21" s="34"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -19851,7 +20231,7 @@
       </c>
       <c r="L22" s="34"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -19888,31 +20268,31 @@
       </c>
       <c r="L23" s="34"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D25" s="15"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I27" s="59"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I28" s="59"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I29" s="59"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I30" s="59"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I31" s="59"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I32" s="59"/>
     </row>
-    <row r="33" spans="9:9">
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I33" s="59"/>
     </row>
-    <row r="34" spans="9:9">
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I34" s="59"/>
     </row>
   </sheetData>
@@ -19933,19 +20313,19 @@
       <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="5" max="5" width="11" style="85" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="85"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" style="85" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="85"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="85" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -19984,7 +20364,7 @@
       </c>
       <c r="M1" s="25"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
         <v>116</v>
       </c>
@@ -20024,7 +20404,7 @@
       </c>
       <c r="M2" s="9"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="68" t="s">
         <v>117</v>
       </c>
@@ -20061,7 +20441,7 @@
       </c>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="68" t="s">
         <v>118</v>
       </c>
@@ -20101,7 +20481,7 @@
       </c>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
         <v>119</v>
       </c>
@@ -20138,7 +20518,7 @@
       </c>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="68" t="s">
         <v>120</v>
       </c>
@@ -20179,7 +20559,7 @@
       </c>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" ht="14.4" customHeight="1">
+    <row r="7" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="68" t="s">
         <v>471</v>
       </c>
@@ -20216,7 +20596,7 @@
       </c>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="J8" s="11"/>
@@ -20224,7 +20604,7 @@
       <c r="L8" s="36"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>122</v>
       </c>
@@ -20264,7 +20644,7 @@
       </c>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>122</v>
       </c>
@@ -20304,7 +20684,7 @@
       </c>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -20344,7 +20724,7 @@
       </c>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -20384,7 +20764,7 @@
       </c>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -20424,7 +20804,7 @@
       </c>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -20464,7 +20844,7 @@
       </c>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -20504,7 +20884,7 @@
       </c>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>127</v>
       </c>
@@ -20544,7 +20924,7 @@
       </c>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>128</v>
       </c>
@@ -20584,7 +20964,7 @@
       </c>
       <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -20624,7 +21004,7 @@
       </c>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>123</v>
       </c>
@@ -20664,7 +21044,7 @@
       </c>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>123</v>
       </c>
@@ -20704,7 +21084,7 @@
       </c>
       <c r="M20" s="9"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>129</v>
       </c>
@@ -20744,7 +21124,7 @@
       </c>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -20784,7 +21164,7 @@
       </c>
       <c r="M22" s="9"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -20824,7 +21204,7 @@
       </c>
       <c r="M23" s="9"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -20864,7 +21244,7 @@
       </c>
       <c r="M24" s="9"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>124</v>
       </c>
@@ -20904,7 +21284,7 @@
       </c>
       <c r="M25" s="9"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>124</v>
       </c>
@@ -20944,7 +21324,7 @@
       </c>
       <c r="M26" s="14"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>131</v>
       </c>
@@ -20984,7 +21364,7 @@
       </c>
       <c r="M27" s="9"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>131</v>
       </c>
@@ -21024,7 +21404,7 @@
       </c>
       <c r="M28" s="9"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>132</v>
       </c>
@@ -21064,7 +21444,7 @@
       </c>
       <c r="M29" s="9"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>132</v>
       </c>
@@ -21104,7 +21484,7 @@
       </c>
       <c r="M30" s="9"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>133</v>
       </c>
@@ -21144,7 +21524,7 @@
       </c>
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>133</v>
       </c>
@@ -21177,7 +21557,7 @@
       <c r="L32" s="36"/>
       <c r="M32" s="9"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="I33" s="55"/>
@@ -21185,7 +21565,7 @@
       <c r="K33" s="55"/>
       <c r="L33" s="55"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>370</v>
       </c>
@@ -21222,7 +21602,7 @@
       </c>
       <c r="M34" s="9"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="55" t="s">
         <v>370</v>
       </c>

</xml_diff>